<commit_message>
-Changing the MCU to STM32G0B1CEU6N -Adding TVS 3.3V -Reviewed version , all finish
</commit_message>
<xml_diff>
--- a/Released/BOM/P01R0.xlsx
+++ b/Released/BOM/P01R0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\P01R0x-Hardware\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANAS\Downloads\P01R0x-Hardware-main\P01R0x-Hardware-main\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7502E100-24A0-45E0-9A43-508A8C689109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="P01R0" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
   <si>
     <t>Description</t>
   </si>
@@ -91,15 +90,9 @@
     <t>Vishay</t>
   </si>
   <si>
-    <t>JP1</t>
-  </si>
-  <si>
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>JP2</t>
-  </si>
-  <si>
     <t>Conn Unshrouded Header HDR 3 POS 2.54mm Solder ST Top Entry Thru-Hole Carton</t>
   </si>
   <si>
@@ -115,9 +108,6 @@
     <t>https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g</t>
   </si>
   <si>
-    <t>YAGEO [VA]</t>
-  </si>
-  <si>
     <t>CC0805KKX7R7BB105</t>
   </si>
   <si>
@@ -130,9 +120,6 @@
     <t>RES SMD 0.0OHM JUMPER 1/10W 0603</t>
   </si>
   <si>
-    <t>YAGEO [VR]</t>
-  </si>
-  <si>
     <t>RC0603JR-070RL</t>
   </si>
   <si>
@@ -295,15 +282,9 @@
     <t>Hexabitz Modules</t>
   </si>
   <si>
-    <t xml:space="preserve"> C7, C4</t>
-  </si>
-  <si>
     <t>C2</t>
   </si>
   <si>
-    <t xml:space="preserve"> C3, C5, C6, C8</t>
-  </si>
-  <si>
     <t>Conn Unshrouded Header HDR 1 POS Solder ST Top Entry Thru-Hole Carton</t>
   </si>
   <si>
@@ -314,17 +295,47 @@
   </si>
   <si>
     <t xml:space="preserve">RGB LED (P01R0) </t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>SWD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C1, C3, C5, C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C4, C7</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>BOURNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bidirectional 3.3 V TVS </t>
+  </si>
+  <si>
+    <t>https://octopart.com/cdsod323-t03sc-bourns-10487153?r=sp</t>
+  </si>
+  <si>
+    <t>CDSOD323-T03SC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -338,7 +349,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -349,21 +360,21 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -376,7 +387,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -397,7 +408,7 @@
     <font>
       <b/>
       <sz val="36"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -410,12 +421,12 @@
     <font>
       <u/>
       <sz val="9"/>
-      <color theme="10"/>
+      <color theme="8"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +436,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -572,16 +589,19 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -604,12 +624,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -985,21 +999,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" customWidth="1"/>
-    <col min="2" max="2" width="53.59765625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.296875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.28515625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1014,7 +1028,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="45.6" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.7">
       <c r="A2" s="7"/>
       <c r="B2" s="17"/>
       <c r="C2" s="9" t="s">
@@ -1040,7 +1054,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1050,43 +1064,43 @@
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="29">
         <v>1</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="29">
-        <v>45321</v>
-      </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31"/>
+      <c r="D5" s="30">
+        <v>45343</v>
+      </c>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="35"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1109,61 +1123,61 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>94</v>
+      <c r="D9" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="F9" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="E10" s="28" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="36" t="s">
-        <v>26</v>
       </c>
       <c r="F10" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>28</v>
+      <c r="D11" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="F11" s="26">
         <v>4</v>
@@ -1171,19 +1185,19 @@
     </row>
     <row r="12" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="36" t="s">
-        <v>31</v>
+        <v>72</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="F12" s="26">
         <v>1</v>
@@ -1191,18 +1205,18 @@
     </row>
     <row r="13" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="26">
@@ -1211,19 +1225,19 @@
     </row>
     <row r="14" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>39</v>
+      <c r="D14" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>35</v>
       </c>
       <c r="F14" s="26">
         <v>1</v>
@@ -1231,19 +1245,19 @@
     </row>
     <row r="15" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="28" t="s">
         <v>32</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>36</v>
       </c>
       <c r="F15" s="26">
         <v>1</v>
@@ -1251,19 +1265,19 @@
     </row>
     <row r="16" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="28" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>41</v>
       </c>
       <c r="F16" s="26">
         <v>1</v>
@@ -1271,19 +1285,19 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>71</v>
+      <c r="E17" s="28" t="s">
+        <v>67</v>
       </c>
       <c r="F17" s="26">
         <v>1</v>
@@ -1291,19 +1305,19 @@
     </row>
     <row r="18" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="28" t="s">
         <v>69</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>73</v>
       </c>
       <c r="F18" s="26">
         <v>2</v>
@@ -1311,119 +1325,119 @@
     </row>
     <row r="19" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>78</v>
+      <c r="D19" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>74</v>
       </c>
       <c r="F19" s="26">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="28" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>46</v>
       </c>
       <c r="F20" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>50</v>
+        <v>43</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>46</v>
       </c>
       <c r="F21" s="26">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="28" t="s">
         <v>51</v>
-      </c>
-      <c r="E22" s="36" t="s">
-        <v>55</v>
       </c>
       <c r="F22" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="15" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="36" t="s">
-        <v>58</v>
+      <c r="D23" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="F23" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="36" t="s">
-        <v>66</v>
+        <v>81</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>62</v>
       </c>
       <c r="F24" s="26">
         <v>1</v>
@@ -1431,21 +1445,41 @@
     </row>
     <row r="25" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="26">
+      <c r="D26" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="26">
         <v>1</v>
       </c>
     </row>
@@ -1456,22 +1490,22 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C24" r:id="rId1" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E17" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E25" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E22" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E20" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E16" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E12" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E21" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C24" r:id="rId1" display="https://octopart.com/manufacturers/wolfspeed"/>
+    <hyperlink ref="E19" r:id="rId2"/>
+    <hyperlink ref="E18" r:id="rId3"/>
+    <hyperlink ref="E10" r:id="rId4"/>
+    <hyperlink ref="E17" r:id="rId5"/>
+    <hyperlink ref="E14" r:id="rId6"/>
+    <hyperlink ref="E26" r:id="rId7"/>
+    <hyperlink ref="E23" r:id="rId8"/>
+    <hyperlink ref="E22" r:id="rId9"/>
+    <hyperlink ref="E20" r:id="rId10"/>
+    <hyperlink ref="E16" r:id="rId11"/>
+    <hyperlink ref="E15" r:id="rId12"/>
+    <hyperlink ref="E13" r:id="rId13"/>
+    <hyperlink ref="E12" r:id="rId14"/>
+    <hyperlink ref="E21" r:id="rId15"/>
+    <hyperlink ref="E11" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>

</xml_diff>

<commit_message>
-Add TVS diode -Change the MCU to STM32G0B1CEU6 -Activate the thermal option for the polygon -Improve the layout design for better appearence
</commit_message>
<xml_diff>
--- a/Released/BOM/P01R0.xlsx
+++ b/Released/BOM/P01R0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANAS\Downloads\P01R0x-Hardware-main\P01R0x-Hardware-main\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moazzen\Downloads\Telegram Desktop\P01R0x-Hardware-main\P01R0x-Hardware-main\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0C3356-FF17-4D0F-B4AB-95DBCADFA3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P01R0" sheetId="1" r:id="rId1"/>
@@ -147,9 +148,6 @@
     <t>Ind chip Bead Multi-Layer 30 ohms 25% 100MHZ Ferrite 1,5A 0603Punched paper T/R</t>
   </si>
   <si>
-    <t xml:space="preserve">TDK </t>
-  </si>
-  <si>
     <t>MMZ1608Y300BTA00</t>
   </si>
   <si>
@@ -168,9 +166,6 @@
     <t>https://octopart.com/mmbt3904lt1g-on+semiconductor-3280?r=sp</t>
   </si>
   <si>
-    <t>STM32G0B1CEU6N</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -180,9 +175,6 @@
     <t>STMicroelectronics</t>
   </si>
   <si>
-    <t>https://octopart.com/stm32g0b1ceu6n-stmicroelectronics-116364672?r=sp</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -303,12 +295,6 @@
     <t>SWD</t>
   </si>
   <si>
-    <t xml:space="preserve">  C1, C3, C5, C6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> C4, C7</t>
-  </si>
-  <si>
     <t>YAGEO</t>
   </si>
   <si>
@@ -318,24 +304,39 @@
     <t>BOURNS</t>
   </si>
   <si>
-    <t xml:space="preserve">Bidirectional 3.3 V TVS </t>
-  </si>
-  <si>
     <t>https://octopart.com/cdsod323-t03sc-bourns-10487153?r=sp</t>
   </si>
   <si>
     <t>CDSOD323-T03SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  C1, C5, C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>TVS DIODE 3,3V 10,9V SOD323</t>
+  </si>
+  <si>
+    <t>STM32G0B1CEU6</t>
+  </si>
+  <si>
+    <t>https://octopart.com/stm32g0b1ceu6-stmicroelectronics-116363364?r=sp</t>
+  </si>
+  <si>
+    <t>TDK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -349,7 +350,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -360,21 +361,21 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -387,7 +388,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -408,7 +409,7 @@
     <font>
       <b/>
       <sz val="36"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -524,7 +525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -545,7 +546,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -660,7 +660,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2174599</xdr:colOff>
+      <xdr:colOff>2470434</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
@@ -999,44 +999,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="53.5703125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.28515625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.296875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="18.296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.19921875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="7.19921875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
-      <c r="B1" s="16"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="16"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:9" ht="45.6" x14ac:dyDescent="0.75">
       <c r="A2" s="7"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="14" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="13" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="5"/>
@@ -1044,442 +1043,442 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="28">
         <v>1</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>84</v>
+      <c r="B5" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <v>45343</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>89</v>
+      <c r="B6" s="18" t="s">
+        <v>86</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="21" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+    <row r="9" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="14" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="26">
+      <c r="B25" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+    <row r="26" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="C26" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="15" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="E26" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="26">
+      <c r="F26" s="25">
         <v>1</v>
       </c>
     </row>
@@ -1490,22 +1489,22 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C24" r:id="rId1" display="https://octopart.com/manufacturers/wolfspeed"/>
-    <hyperlink ref="E19" r:id="rId2"/>
-    <hyperlink ref="E18" r:id="rId3"/>
-    <hyperlink ref="E10" r:id="rId4"/>
-    <hyperlink ref="E17" r:id="rId5"/>
-    <hyperlink ref="E14" r:id="rId6"/>
-    <hyperlink ref="E26" r:id="rId7"/>
-    <hyperlink ref="E23" r:id="rId8"/>
-    <hyperlink ref="E22" r:id="rId9"/>
-    <hyperlink ref="E20" r:id="rId10"/>
-    <hyperlink ref="E16" r:id="rId11"/>
-    <hyperlink ref="E15" r:id="rId12"/>
-    <hyperlink ref="E13" r:id="rId13"/>
-    <hyperlink ref="E12" r:id="rId14"/>
-    <hyperlink ref="E21" r:id="rId15"/>
-    <hyperlink ref="E11" r:id="rId16"/>
+    <hyperlink ref="C24" r:id="rId1" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E17" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E26" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E12" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E21" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E22" r:id="rId16" xr:uid="{316D9BDC-9582-46F6-91C2-3B0F541B4580}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>

</xml_diff>